<commit_message>
Searchbar and checkox added
</commit_message>
<xml_diff>
--- a/Files/Test Plan for Professional Practices.xlsx
+++ b/Files/Test Plan for Professional Practices.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="69">
   <si>
     <t>Purpose:</t>
   </si>
@@ -247,13 +247,23 @@
   </si>
   <si>
     <t>1. Launch Home page
-2. Clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user can clear the potholes on the map by clicking the select box in the top left side of the map </t>
-  </si>
-  <si>
-    <t>The user clicks the clear button up the top left corner of the map, and all the potholes markers are removed</t>
+2. CheckBox</t>
+  </si>
+  <si>
+    <t>The user can click a checkbox in the top right hand corner of the map. This will allow an admin to see where the most frequent spots for accidents are, over the past 2 weeks</t>
+  </si>
+  <si>
+    <t>1. Launch Home page
+2. SearchBar</t>
+  </si>
+  <si>
+    <t>The user can click into the searchbar at the top of the application, where they can enter a location to see if there's any accidents or potholes heading towards their desired destination</t>
+  </si>
+  <si>
+    <t>The user clicks the searchbar, where they enter their desired location to see if there's any accident or potholes along the way</t>
+  </si>
+  <si>
+    <t>The user clicks the checkbox, and the map will display where all accident markers have been, over the past 2 weeks</t>
   </si>
 </sst>
 </file>
@@ -490,7 +500,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="57">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1171,7 +1202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -1834,25 +1865,45 @@
         <v>64</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="8"/>
+    <row r="21" spans="1:12" s="10" customFormat="1" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9">
+        <v>1</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
     </row>
@@ -1977,191 +2028,202 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:F2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J1:J4 J21:J1048576">
-    <cfRule type="containsText" dxfId="53" priority="58" operator="containsText" text="Invalid Test">
+  <conditionalFormatting sqref="J1:J4 J22:J1048576">
+    <cfRule type="containsText" dxfId="56" priority="61" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="55" priority="62" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="54" priority="63" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="containsText" dxfId="50" priority="55" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="53" priority="58" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="56" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="57" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",J20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",J20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",J20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Invalid Test">
-      <formula>NOT(ISERROR(SEARCH("Invalid Test",J20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",J21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",J20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",J21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",J20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pass",J21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>